<commit_message>
updates to the draft
</commit_message>
<xml_diff>
--- a/nesh/lambda calculations with revised sigma_m.xlsx
+++ b/nesh/lambda calculations with revised sigma_m.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nesh/Documents/Repositories/icecontinuum/nesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1932EA70-D650-144E-AA14-E52B408B0B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC97A10-DA68-3D43-B464-8165CEEE621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
+    <workbookView xWindow="2160" yWindow="500" windowWidth="26640" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>D (um^2/us)</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Unstable runs</t>
   </si>
   <si>
-    <t>lambda seems insensitive to tau</t>
-  </si>
-  <si>
     <t>nu_kin (um/s)</t>
   </si>
   <si>
@@ -91,13 +88,28 @@
     <t>exp of D</t>
   </si>
   <si>
-    <t>nx changed proportionally, so dx=0.3</t>
-  </si>
-  <si>
     <t>LSODA integrator, dx=.3 um</t>
   </si>
   <si>
     <t>I think this is borderline stable/unstable -- the lambda is lower than the value at sigmaIcorner = 0.21, which bucks the trend</t>
+  </si>
+  <si>
+    <t>This is smallest D before going unstable</t>
+  </si>
+  <si>
+    <t>This is the smallest c_r I tried</t>
+  </si>
+  <si>
+    <t>This is the largest nu_kin I tried</t>
+  </si>
+  <si>
+    <t>This is the biggest c_r I tried</t>
+  </si>
+  <si>
+    <t>This is the biggest D I tried</t>
+  </si>
+  <si>
+    <t>This is the smallest nu_kin I tried</t>
   </si>
 </sst>
 </file>
@@ -131,10 +143,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial Unicode MS"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -165,18 +179,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,7 +251,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.4143565194233407E-2"/>
+          <c:y val="6.8377794197272981E-2"/>
+          <c:w val="0.89158996422447667"/>
+          <c:h val="0.71002898895748623"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -315,84 +336,90 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.32659863237109038</c:v>
+                  <c:v>1.0846522890932808</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.76696498884737041</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7149858514250884</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54232614454664041</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.34299717028501764</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.34299717028501764</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.48507125007266588</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.48507125007266588</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48507125007266588</c:v>
+                  <c:v>0.30678599553894814</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.76696498884737041</c:v>
+                  <c:v>2.4253562503633295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76696498884737052</c:v>
+                  <c:v>3.4299717028501764</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.76696498884737052</c:v>
+                  <c:v>0.63245553203367577</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0846522890932808</c:v>
+                  <c:v>0.44721359549995787</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4142135623730949</c:v>
+                  <c:v>0.36514837167011066</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6329931618554518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$12</c:f>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3.0120481927710845</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>9.9469496021220163</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2751091703056772</c:v>
+                  <c:v>6.9637883008356551</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3333333333333335</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.6875</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.8701298701298699</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0675675675675675</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.7319587628865989</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.7922077922077921</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.775862068965518</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.423076923076923</c:v>
+                  <c:v>15.789473684210526</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0">
+                  <c:v>4.9570389953734297</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0">
+                  <c:v>3.0537459283387625</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0">
+                  <c:v>2.7056277056277058</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0">
+                  <c:v>22.255192878338278</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0">
+                  <c:v>31.380753138075313</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0">
+                  <c:v>5.4744525547445262</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0">
+                  <c:v>3.5561877667140824</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0">
+                  <c:v>2.6483050847457625</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.0">
+                  <c:v>15.306122448979592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -500,7 +527,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -609,7 +636,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9643741685561293E-2"/>
+          <c:y val="4.2317684606213331E-2"/>
+          <c:w val="0.92115309205169371"/>
+          <c:h val="0.90955053079330039"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -640,12 +677,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$40</c:f>
+              <c:f>Sheet1!$B$28:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.6</c:v>
@@ -672,94 +709,88 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.01</c:v>
+                  <c:v>-0.02</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.02</c:v>
+                  <c:v>-0.03</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.03</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.05</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.1</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.2</c:v>
+                  <c:v>-0.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.3</c:v>
+                  <c:v>-0.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.45</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$23:$E$40</c:f>
+              <c:f>Sheet1!$E$28:$E$44</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>2.7075812274368234</c:v>
+                  <c:v>2.6910656620021527</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1073384446878416</c:v>
+                  <c:v>3.2808398950131235</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1983471074380168</c:v>
+                  <c:v>5.3686471009305654</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4269662921348303</c:v>
+                  <c:v>7.5225677031093277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1463414634146343</c:v>
+                  <c:v>8.2964601769911503</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>9.1687041564792171</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.714285714285714</c:v>
+                  <c:v>9.8039215686274499</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.9469496021220163</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.261261261261261</c:v>
+                  <c:v>9.5785440613026811</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.117647058823529</c:v>
+                  <c:v>33.185840707964601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.185840707964601</c:v>
+                  <c:v>27.272727272727273</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.075812274368232</c:v>
+                  <c:v>20.491803278688522</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.161290322580644</c:v>
+                  <c:v>13.089005235602093</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.396694214876034</c:v>
+                  <c:v>7.6844262295081966</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.756756756756757</c:v>
+                  <c:v>5.3724928366762175</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.4117647058823533</c:v>
+                  <c:v>4.0805223068552774</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0612244897959182</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.5938566552901023</c:v>
+                  <c:v>3.288619645175249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -868,7 +899,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2083,10 +2114,10 @@
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>92029</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2113,16 +2144,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>21345</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>886417</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>58438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>74706</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>59358</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>56301</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2447,11 +2478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FACA8F-BEA8-A344-9B24-B4206D9D79F6}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2459,9 +2490,10 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="13"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="13" customWidth="1"/>
     <col min="11" max="12" width="13.33203125" customWidth="1"/>
     <col min="13" max="13" width="16.5" customWidth="1"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
@@ -2469,7 +2501,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -2477,7 +2509,7 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -2486,7 +2518,7 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
@@ -2499,68 +2531,68 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B2" s="7">
-        <f>F2^$C$14*C2^$C$17*K2^$C$16*I2^$C$15*10</f>
-        <v>0.32659863237109038</v>
-      </c>
-      <c r="C2" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <f>F2^$C$19*C2^$C$22*K2^$C$21*I2^$C$20*10</f>
+        <v>1.0846522890932808</v>
+      </c>
+      <c r="C2">
         <v>75</v>
       </c>
-      <c r="D2" s="9">
-        <v>24.9</v>
-      </c>
-      <c r="E2" s="9">
-        <f t="shared" ref="E2:E12" si="0">C2/D2</f>
-        <v>3.0120481927710845</v>
-      </c>
-      <c r="F2" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="D2" s="15">
+        <v>7.54</v>
+      </c>
+      <c r="E2" s="5">
+        <f t="shared" ref="E2" si="0">C2/D2</f>
+        <v>9.9469496021220163</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H2">
         <v>0.2</v>
       </c>
-      <c r="H2" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I2" s="18">
+      <c r="I2" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J2" s="8">
         <v>1</v>
       </c>
       <c r="K2" s="8">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B3" s="7">
-        <f t="shared" ref="B3:B12" si="1">F3^$C$14*C3^$C$17*K3^$C$16*I3^$C$15*10</f>
-        <v>0.34299717028501764</v>
+      <c r="B3" s="9">
+        <f>F3^$C$19*C3^$C$22*K3^$C$21*I3^$C$20*10</f>
+        <v>0.76696498884737041</v>
       </c>
       <c r="C3" s="8">
         <v>75</v>
       </c>
-      <c r="D3" s="9">
-        <v>22.9</v>
-      </c>
-      <c r="E3" s="9">
-        <f t="shared" si="0"/>
-        <v>3.2751091703056772</v>
-      </c>
-      <c r="F3" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="D3" s="15">
+        <v>10.77</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E5" si="1">C3/D3</f>
+        <v>6.9637883008356551</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H3">
         <v>0.2</v>
       </c>
-      <c r="H3" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I3" s="18">
+      <c r="I3" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J3" s="8">
@@ -2569,33 +2601,36 @@
       <c r="K3" s="8">
         <v>34</v>
       </c>
+      <c r="L3" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.34299717028501764</v>
+      <c r="B4" s="9">
+        <f>F4^$C$19*C4^$C$22*K4^$C$21*I4^$C$20*10</f>
+        <v>1.7149858514250884</v>
       </c>
       <c r="C4" s="8">
         <v>75</v>
       </c>
-      <c r="D4" s="9">
-        <v>22.5</v>
-      </c>
-      <c r="E4" s="9">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="F4" s="11">
-        <v>1E-4</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="D4" s="15">
+        <v>4.75</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="1"/>
+        <v>15.789473684210526</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H4" s="8">
         <v>0.2</v>
       </c>
-      <c r="H4" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I4" s="18">
-        <v>2.5000000000000001E-3</v>
+      <c r="I4" s="6">
+        <v>1E-3</v>
       </c>
       <c r="J4" s="8">
         <v>1</v>
@@ -2604,32 +2639,32 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+    <row r="5" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <f t="shared" ref="B5" si="2">F5^$C$19*C5^$C$22*K5^$C$21*I5^$C$20*10</f>
+        <v>0.54232614454664041</v>
+      </c>
+      <c r="C5">
+        <v>75</v>
+      </c>
+      <c r="D5" s="15">
+        <v>15.13</v>
+      </c>
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>0.48507125007266588</v>
-      </c>
-      <c r="C5" s="8">
-        <v>75</v>
-      </c>
-      <c r="D5" s="9">
-        <v>16</v>
-      </c>
-      <c r="E5" s="9">
-        <f t="shared" si="0"/>
-        <v>4.6875</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G5" s="7">
+        <v>4.9570389953734297</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H5">
         <v>0.2</v>
       </c>
-      <c r="H5" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I5" s="18">
-        <v>2.5000000000000001E-3</v>
+      <c r="I5" s="1">
+        <v>1E-3</v>
       </c>
       <c r="J5" s="8">
         <v>1</v>
@@ -2637,106 +2672,109 @@
       <c r="K5" s="8">
         <v>34</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="L5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
-        <f t="shared" si="1"/>
-        <v>0.48507125007266588</v>
+      <c r="B6" s="9">
+        <f t="shared" ref="B6" si="3">F6^$C$19*C6^$C$22*K6^$C$21*I6^$C$20*10</f>
+        <v>0.34299717028501764</v>
       </c>
       <c r="C6" s="8">
         <v>75</v>
       </c>
-      <c r="D6" s="9">
-        <v>15.4</v>
-      </c>
-      <c r="E6" s="9">
-        <f t="shared" si="0"/>
-        <v>4.8701298701298699</v>
-      </c>
-      <c r="F6" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="D6" s="15">
+        <v>24.56</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" ref="E6" si="4">C6/D6</f>
+        <v>3.0537459283387625</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H6" s="8">
         <v>0.2</v>
       </c>
-      <c r="H6" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I6" s="18">
+      <c r="I6" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J6" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K6" s="8">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
-        <f t="shared" si="1"/>
-        <v>0.48507125007266588</v>
+      <c r="B7" s="9">
+        <f t="shared" ref="B7:B8" si="5">F7^$C$19*C7^$C$22*K7^$C$21*I7^$C$20*10</f>
+        <v>0.30678599553894814</v>
       </c>
       <c r="C7" s="8">
         <v>75</v>
       </c>
-      <c r="D7" s="9">
-        <v>14.8</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" si="0"/>
-        <v>5.0675675675675675</v>
-      </c>
-      <c r="F7" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="D7" s="15">
+        <v>27.72</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" ref="E7:E8" si="6">C7/D7</f>
+        <v>2.7056277056277058</v>
+      </c>
+      <c r="F7" s="12">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H7" s="8">
         <v>0.2</v>
       </c>
-      <c r="H7" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I7" s="18">
+      <c r="I7" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J7" s="8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="8">
         <v>34</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
-        <f t="shared" si="1"/>
-        <v>0.76696498884737041</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="L7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <f t="shared" si="5"/>
+        <v>2.4253562503633295</v>
+      </c>
+      <c r="C8">
         <v>75</v>
       </c>
-      <c r="D8" s="9">
-        <v>10</v>
-      </c>
-      <c r="E8" s="9">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="F8" s="11">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="D8" s="15">
+        <v>3.37</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="6"/>
+        <v>22.255192878338278</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H8">
         <v>0.2</v>
       </c>
-      <c r="H8" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I8" s="18">
+      <c r="I8" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J8" s="8">
@@ -2745,36 +2783,36 @@
       <c r="K8" s="8">
         <v>34</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <f t="shared" si="1"/>
-        <v>0.76696498884737052</v>
-      </c>
-      <c r="C9" s="8">
+    <row r="9" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <f t="shared" ref="B9:B10" si="7">F9^$C$19*C9^$C$22*K9^$C$21*I9^$C$20*10</f>
+        <v>3.4299717028501764</v>
+      </c>
+      <c r="C9">
         <v>75</v>
       </c>
-      <c r="D9" s="9">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="E9" s="9">
-        <f t="shared" si="0"/>
-        <v>7.7319587628865989</v>
-      </c>
-      <c r="F9" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="D9" s="15">
+        <v>2.39</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ref="E9:E10" si="8">C9/D9</f>
+        <v>31.380753138075313</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H9">
         <v>0.2</v>
       </c>
-      <c r="H9" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I9" s="18">
-        <v>1E-3</v>
+      <c r="I9" s="1">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="J9" s="8">
         <v>1</v>
@@ -2782,357 +2820,279 @@
       <c r="K9" s="8">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
-        <f t="shared" si="1"/>
-        <v>0.76696498884737052</v>
-      </c>
-      <c r="C10" s="8">
-        <v>120</v>
-      </c>
-      <c r="D10" s="9">
-        <v>15.4</v>
-      </c>
-      <c r="E10" s="9">
-        <f t="shared" si="0"/>
-        <v>7.7922077922077921</v>
-      </c>
-      <c r="F10" s="11">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="L9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <f t="shared" si="7"/>
+        <v>0.63245553203367577</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10" s="15">
+        <v>13.7</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="8"/>
+        <v>5.4744525547445262</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H10">
         <v>0.2</v>
       </c>
-      <c r="H10" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I10" s="18">
-        <v>1E-3</v>
+      <c r="I10" s="1">
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="J10" s="8">
         <v>1</v>
       </c>
       <c r="K10" s="8">
-        <v>34</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
-        <f t="shared" si="1"/>
-        <v>1.0846522890932808</v>
-      </c>
-      <c r="C11" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <f t="shared" ref="B11" si="9">F11^$C$19*C11^$C$22*K11^$C$21*I11^$C$20*10</f>
+        <v>0.44721359549995787</v>
+      </c>
+      <c r="C11">
         <v>75</v>
       </c>
-      <c r="D11" s="9">
-        <v>6.96</v>
-      </c>
-      <c r="E11" s="9">
-        <f t="shared" si="0"/>
-        <v>10.775862068965518</v>
-      </c>
-      <c r="F11" s="11">
+      <c r="D11" s="15">
+        <v>21.09</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11" si="10">C11/D11</f>
+        <v>3.5561877667140824</v>
+      </c>
+      <c r="F11" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H11">
         <v>0.2</v>
       </c>
-      <c r="H11" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I11" s="18">
+      <c r="I11" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J11" s="8">
         <v>1</v>
       </c>
       <c r="K11" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-      <c r="C12" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <f t="shared" ref="B12" si="11">F12^$C$19*C12^$C$22*K12^$C$21*I12^$C$20*10</f>
+        <v>0.36514837167011066</v>
+      </c>
+      <c r="C12">
         <v>75</v>
       </c>
-      <c r="D12" s="9">
-        <v>5.2</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>14.423076923076923</v>
-      </c>
-      <c r="F12" s="11">
+      <c r="D12" s="15">
+        <v>28.32</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" ref="E12" si="12">C12/D12</f>
+        <v>2.6483050847457625</v>
+      </c>
+      <c r="F12" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H12">
         <v>0.2</v>
       </c>
-      <c r="H12" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="I12" s="18">
+      <c r="I12" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J12" s="8">
         <v>1</v>
       </c>
       <c r="K12" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>300</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <f t="shared" ref="B13" si="13">F13^$C$19*C13^$C$22*K13^$C$21*I13^$C$20*10</f>
+        <v>1.6329931618554518</v>
+      </c>
+      <c r="C13">
+        <v>75</v>
+      </c>
+      <c r="D13" s="15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ref="E13" si="14">C13/D13</f>
+        <v>15.306122448979592</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H13">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8">
+        <v>15</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="14"/>
+      <c r="H15"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="14"/>
+      <c r="H16"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="14"/>
+      <c r="H17"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="14"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="14"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C15">
+      <c r="C20">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17">
+      <c r="C22">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
-        <f t="shared" ref="B23:B40" si="2">G23</f>
-        <v>0.9</v>
-      </c>
-      <c r="C23" s="8">
-        <v>75</v>
-      </c>
-      <c r="D23" s="9">
-        <v>27.7</v>
-      </c>
-      <c r="E23" s="10">
-        <f t="shared" ref="E23:E40" si="3">C23/D23</f>
-        <v>2.7075812274368234</v>
-      </c>
-      <c r="F23" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="G23" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="H23" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I23" s="12">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J23" s="8">
-        <v>1</v>
-      </c>
-      <c r="K23" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
-        <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-      <c r="C24" s="8">
-        <v>75</v>
-      </c>
-      <c r="D24" s="9">
-        <v>18.260000000000002</v>
-      </c>
-      <c r="E24" s="10">
-        <f t="shared" si="3"/>
-        <v>4.1073384446878416</v>
-      </c>
-      <c r="F24" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="G24" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I24" s="12">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J24" s="8">
-        <v>1</v>
-      </c>
-      <c r="K24" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-      <c r="C25" s="8">
-        <v>75</v>
-      </c>
-      <c r="D25" s="9">
-        <v>12.1</v>
-      </c>
-      <c r="E25" s="10">
-        <f t="shared" si="3"/>
-        <v>6.1983471074380168</v>
-      </c>
-      <c r="F25" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="G25" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="H25" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I25" s="12">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J25" s="8">
-        <v>1</v>
-      </c>
-      <c r="K25" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B26" s="7">
-        <f t="shared" si="2"/>
-        <v>0.3</v>
-      </c>
-      <c r="C26" s="8">
-        <v>75</v>
-      </c>
-      <c r="D26" s="9">
-        <v>8.9</v>
-      </c>
-      <c r="E26" s="10">
-        <f t="shared" si="3"/>
-        <v>8.4269662921348303</v>
-      </c>
-      <c r="F26" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="G26" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="H26" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I26" s="12">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J26" s="8">
-        <v>1</v>
-      </c>
-      <c r="K26" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
-        <f t="shared" si="2"/>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="C27" s="8">
-        <v>75</v>
-      </c>
-      <c r="D27" s="9">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E27" s="10">
-        <f t="shared" si="3"/>
-        <v>9.1463414634146343</v>
-      </c>
-      <c r="F27" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="G27" s="7">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="H27" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I27" s="12">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J27" s="8">
-        <v>1</v>
-      </c>
-      <c r="K27" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
+    <row r="28" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B28" s="9">
+        <f t="shared" ref="B28:B44" si="15">G28</f>
+        <v>0.7</v>
       </c>
       <c r="C28" s="8">
         <v>75</v>
       </c>
-      <c r="D28" s="9">
-        <v>7.5</v>
+      <c r="D28" s="15">
+        <v>27.87</v>
       </c>
       <c r="E28" s="10">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="F28" s="11">
+        <f t="shared" ref="E28:E44" si="16">C28/D28</f>
+        <v>2.6910656620021527</v>
+      </c>
+      <c r="F28" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G28" s="7">
-        <v>0.25</v>
+      <c r="G28" s="14">
+        <v>0.7</v>
       </c>
       <c r="H28" s="8">
         <v>0.2</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J28" s="8">
@@ -3142,31 +3102,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
-        <f t="shared" si="2"/>
-        <v>0.23</v>
+    <row r="29" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B29" s="9">
+        <f t="shared" si="15"/>
+        <v>0.6</v>
       </c>
       <c r="C29" s="8">
         <v>75</v>
       </c>
-      <c r="D29" s="9">
-        <v>7</v>
+      <c r="D29" s="15">
+        <v>22.86</v>
       </c>
       <c r="E29" s="10">
-        <f t="shared" si="3"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F29" s="11">
+        <f t="shared" si="16"/>
+        <v>3.2808398950131235</v>
+      </c>
+      <c r="F29" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G29" s="7">
-        <v>0.23</v>
+      <c r="G29" s="14">
+        <v>0.6</v>
       </c>
       <c r="H29" s="8">
         <v>0.2</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J29" s="8">
@@ -3176,65 +3136,65 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="2:11" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B30" s="13">
-        <f t="shared" si="2"/>
-        <v>0.22</v>
-      </c>
-      <c r="C30" s="14">
+    <row r="30" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B30" s="9">
+        <f t="shared" si="15"/>
+        <v>0.4</v>
+      </c>
+      <c r="C30" s="8">
         <v>75</v>
       </c>
       <c r="D30" s="15">
-        <v>7.54</v>
-      </c>
-      <c r="E30" s="16">
-        <f t="shared" si="3"/>
-        <v>9.9469496021220163</v>
-      </c>
-      <c r="F30" s="17">
+        <v>13.97</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="16"/>
+        <v>5.3686471009305654</v>
+      </c>
+      <c r="F30" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G30" s="13">
-        <v>0.22</v>
-      </c>
-      <c r="H30" s="14">
+      <c r="G30" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="H30" s="8">
         <v>0.2</v>
       </c>
       <c r="I30" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="8">
         <v>1</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="8">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
-        <f t="shared" si="2"/>
-        <v>0.21</v>
+    <row r="31" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B31" s="9">
+        <f t="shared" si="15"/>
+        <v>0.3</v>
       </c>
       <c r="C31" s="8">
         <v>75</v>
       </c>
-      <c r="D31" s="9">
-        <v>6.66</v>
+      <c r="D31" s="15">
+        <v>9.9700000000000006</v>
       </c>
       <c r="E31" s="10">
-        <f t="shared" si="3"/>
-        <v>11.261261261261261</v>
-      </c>
-      <c r="F31" s="11">
+        <f t="shared" si="16"/>
+        <v>7.5225677031093277</v>
+      </c>
+      <c r="F31" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G31" s="7">
-        <v>0.21</v>
+      <c r="G31" s="14">
+        <v>0.3</v>
       </c>
       <c r="H31" s="8">
         <v>0.2</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J31" s="8">
@@ -3244,31 +3204,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B32" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.01</v>
+    <row r="32" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B32" s="9">
+        <f t="shared" si="15"/>
+        <v>0.27500000000000002</v>
       </c>
       <c r="C32" s="8">
         <v>75</v>
       </c>
-      <c r="D32" s="9">
-        <v>1.7</v>
+      <c r="D32" s="15">
+        <v>9.0399999999999991</v>
       </c>
       <c r="E32" s="10">
-        <f t="shared" si="3"/>
-        <v>44.117647058823529</v>
-      </c>
-      <c r="F32" s="11">
+        <f t="shared" si="16"/>
+        <v>8.2964601769911503</v>
+      </c>
+      <c r="F32" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G32" s="7">
-        <v>-0.01</v>
+      <c r="G32" s="14">
+        <v>0.27500000000000002</v>
       </c>
       <c r="H32" s="8">
         <v>0.2</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J32" s="8">
@@ -3278,31 +3238,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B33" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.02</v>
+    <row r="33" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
+        <f t="shared" si="15"/>
+        <v>0.25</v>
       </c>
       <c r="C33" s="8">
         <v>75</v>
       </c>
-      <c r="D33" s="9">
-        <v>2.2599999999999998</v>
+      <c r="D33" s="15">
+        <v>8.18</v>
       </c>
       <c r="E33" s="10">
-        <f t="shared" si="3"/>
-        <v>33.185840707964601</v>
-      </c>
-      <c r="F33" s="11">
+        <f t="shared" si="16"/>
+        <v>9.1687041564792171</v>
+      </c>
+      <c r="F33" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G33" s="7">
-        <v>-0.02</v>
+      <c r="G33" s="14">
+        <v>0.25</v>
       </c>
       <c r="H33" s="8">
         <v>0.2</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J33" s="8">
@@ -3312,31 +3272,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B34" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.03</v>
+    <row r="34" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B34" s="9">
+        <f t="shared" si="15"/>
+        <v>0.23</v>
       </c>
       <c r="C34" s="8">
         <v>75</v>
       </c>
-      <c r="D34" s="9">
-        <v>2.77</v>
+      <c r="D34" s="15">
+        <v>7.65</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="3"/>
-        <v>27.075812274368232</v>
-      </c>
-      <c r="F34" s="11">
+        <f t="shared" si="16"/>
+        <v>9.8039215686274499</v>
+      </c>
+      <c r="F34" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G34" s="7">
-        <v>-0.03</v>
+      <c r="G34" s="14">
+        <v>0.23</v>
       </c>
       <c r="H34" s="8">
         <v>0.2</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J34" s="8">
@@ -3346,65 +3306,65 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.05</v>
-      </c>
-      <c r="C35" s="8">
+    <row r="35" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <f t="shared" si="15"/>
+        <v>0.22</v>
+      </c>
+      <c r="C35">
         <v>75</v>
       </c>
-      <c r="D35" s="9">
-        <v>3.72</v>
-      </c>
-      <c r="E35" s="10">
-        <f t="shared" si="3"/>
-        <v>20.161290322580644</v>
-      </c>
-      <c r="F35" s="11">
+      <c r="D35" s="15">
+        <v>7.54</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="16"/>
+        <v>9.9469496021220163</v>
+      </c>
+      <c r="F35" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G35" s="7">
-        <v>-0.05</v>
-      </c>
-      <c r="H35" s="8">
+      <c r="G35" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="H35">
         <v>0.2</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J35">
         <v>1</v>
       </c>
-      <c r="K35" s="8">
+      <c r="K35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B36" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.1</v>
+    <row r="36" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B36" s="9">
+        <f t="shared" si="15"/>
+        <v>0.21</v>
       </c>
       <c r="C36" s="8">
         <v>75</v>
       </c>
-      <c r="D36" s="9">
-        <v>6.05</v>
+      <c r="D36" s="15">
+        <v>7.83</v>
       </c>
       <c r="E36" s="10">
-        <f t="shared" si="3"/>
-        <v>12.396694214876034</v>
-      </c>
-      <c r="F36" s="11">
+        <f t="shared" si="16"/>
+        <v>9.5785440613026811</v>
+      </c>
+      <c r="F36" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G36" s="7">
-        <v>-0.1</v>
+      <c r="G36" s="14">
+        <v>0.21</v>
       </c>
       <c r="H36" s="8">
         <v>0.2</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J36" s="8">
@@ -3414,31 +3374,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.2</v>
+    <row r="37" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B37" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.02</v>
       </c>
       <c r="C37" s="8">
         <v>75</v>
       </c>
-      <c r="D37" s="9">
-        <v>11.1</v>
+      <c r="D37" s="15">
+        <v>2.2599999999999998</v>
       </c>
       <c r="E37" s="10">
-        <f t="shared" si="3"/>
-        <v>6.756756756756757</v>
-      </c>
-      <c r="F37" s="11">
+        <f t="shared" si="16"/>
+        <v>33.185840707964601</v>
+      </c>
+      <c r="F37" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G37" s="7">
-        <v>-0.2</v>
+      <c r="G37" s="14">
+        <v>-0.02</v>
       </c>
       <c r="H37" s="8">
         <v>0.2</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J37" s="8">
@@ -3448,31 +3408,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.3</v>
+    <row r="38" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B38" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.03</v>
       </c>
       <c r="C38" s="8">
         <v>75</v>
       </c>
-      <c r="D38" s="9">
-        <v>17</v>
+      <c r="D38" s="15">
+        <v>2.75</v>
       </c>
       <c r="E38" s="10">
-        <f t="shared" si="3"/>
-        <v>4.4117647058823533</v>
-      </c>
-      <c r="F38" s="11">
+        <f t="shared" si="16"/>
+        <v>27.272727272727273</v>
+      </c>
+      <c r="F38" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G38" s="7">
-        <v>-0.3</v>
+      <c r="G38" s="14">
+        <v>-0.03</v>
       </c>
       <c r="H38" s="8">
         <v>0.2</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J38" s="8">
@@ -3482,31 +3442,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B39" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.4</v>
+    <row r="39" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B39" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.05</v>
       </c>
       <c r="C39" s="8">
         <v>75</v>
       </c>
-      <c r="D39" s="9">
-        <v>24.5</v>
+      <c r="D39" s="15">
+        <v>3.66</v>
       </c>
       <c r="E39" s="10">
-        <f t="shared" si="3"/>
-        <v>3.0612244897959182</v>
-      </c>
-      <c r="F39" s="11">
+        <f t="shared" si="16"/>
+        <v>20.491803278688522</v>
+      </c>
+      <c r="F39" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G39" s="7">
-        <v>-0.4</v>
+      <c r="G39" s="14">
+        <v>-0.05</v>
       </c>
       <c r="H39" s="8">
         <v>0.2</v>
       </c>
-      <c r="I39" s="12">
+      <c r="I39" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="J39" s="8">
@@ -3516,163 +3476,192 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B40" s="7">
-        <f t="shared" si="2"/>
-        <v>-0.45</v>
+    <row r="40" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B40" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.1</v>
       </c>
       <c r="C40" s="8">
-        <v>76</v>
-      </c>
-      <c r="D40" s="9">
-        <v>29.3</v>
+        <v>75</v>
+      </c>
+      <c r="D40" s="15">
+        <v>5.73</v>
       </c>
       <c r="E40" s="10">
-        <f t="shared" si="3"/>
-        <v>2.5938566552901023</v>
-      </c>
-      <c r="F40" s="11">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="G40" s="7">
-        <v>-0.45</v>
+        <f t="shared" si="16"/>
+        <v>13.089005235602093</v>
+      </c>
+      <c r="F40" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G40" s="14">
+        <v>-0.1</v>
       </c>
       <c r="H40" s="8">
         <v>0.2</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="3"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="C44">
+      <c r="J40" s="8">
+        <v>1</v>
+      </c>
+      <c r="K40" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B41" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.2</v>
+      </c>
+      <c r="C41" s="8">
         <v>75</v>
       </c>
-      <c r="F44" s="2">
+      <c r="D41" s="15">
+        <v>9.76</v>
+      </c>
+      <c r="E41" s="10">
+        <f t="shared" si="16"/>
+        <v>7.6844262295081966</v>
+      </c>
+      <c r="F41" s="12">
         <v>1E-3</v>
       </c>
-      <c r="G44">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="H44">
-        <v>0.19</v>
+      <c r="G41" s="14">
+        <v>-0.2</v>
+      </c>
+      <c r="H41" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J41" s="8">
+        <v>1</v>
+      </c>
+      <c r="K41" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B42" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.3</v>
+      </c>
+      <c r="C42" s="8">
+        <v>75</v>
+      </c>
+      <c r="D42" s="15">
+        <v>13.96</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="16"/>
+        <v>5.3724928366762175</v>
+      </c>
+      <c r="F42" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G42" s="14">
+        <v>-0.3</v>
+      </c>
+      <c r="H42" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="I42" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J42" s="8">
+        <v>1</v>
+      </c>
+      <c r="K42" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B43" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.4</v>
+      </c>
+      <c r="C43" s="8">
+        <v>75</v>
+      </c>
+      <c r="D43" s="15">
+        <v>18.38</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="16"/>
+        <v>4.0805223068552774</v>
+      </c>
+      <c r="F43" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G43" s="14">
+        <v>-0.4</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J43" s="8">
+        <v>1</v>
+      </c>
+      <c r="K43" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="9">
+        <f t="shared" si="15"/>
+        <v>-0.5</v>
+      </c>
+      <c r="C44" s="8">
+        <v>76</v>
+      </c>
+      <c r="D44" s="15">
+        <v>23.11</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="16"/>
+        <v>3.288619645175249</v>
+      </c>
+      <c r="F44" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G44" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0.2</v>
       </c>
       <c r="I44" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="K44">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="B45" s="5"/>
-      <c r="C45">
-        <v>75</v>
-      </c>
-      <c r="F45" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="G45">
-        <v>0.192</v>
-      </c>
-      <c r="H45">
-        <v>0.19</v>
-      </c>
-      <c r="I45" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
-      <c r="C46">
-        <v>75</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="G46" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="H46">
-        <v>0.19</v>
-      </c>
-      <c r="I46" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-      <c r="K46">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-      <c r="C47">
-        <v>75</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="H47">
-        <v>0.19</v>
-      </c>
-      <c r="I47" s="1">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="J47">
-        <v>1</v>
-      </c>
-      <c r="K47">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
+    </row>
+    <row r="45" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="14"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="17" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>75</v>
       </c>
-      <c r="D48" s="4">
-        <v>6.91</v>
-      </c>
-      <c r="E48" s="5">
-        <f>C48/D48</f>
-        <v>10.85383502170767</v>
-      </c>
       <c r="F48" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G48" s="3">
-        <v>0.2</v>
+      <c r="G48" s="13">
+        <v>0.19400000000000001</v>
       </c>
       <c r="H48">
         <v>0.19</v>
@@ -3686,13 +3675,120 @@
       <c r="K48">
         <v>34</v>
       </c>
-      <c r="L48" t="s">
-        <v>20</v>
+    </row>
+    <row r="49" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="C49">
+        <v>75</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G49" s="13">
+        <v>0.192</v>
+      </c>
+      <c r="H49">
+        <v>0.19</v>
+      </c>
+      <c r="I49" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50">
+        <v>75</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G50" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="H50">
+        <v>0.19</v>
+      </c>
+      <c r="I50" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51">
+        <v>75</v>
+      </c>
+      <c r="D51" s="15"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G51" s="14">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H51">
+        <v>0.19</v>
+      </c>
+      <c r="I51" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52">
+        <v>75</v>
+      </c>
+      <c r="D52" s="15">
+        <v>6.91</v>
+      </c>
+      <c r="E52" s="5">
+        <f>C52/D52</f>
+        <v>10.85383502170767</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G52" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H52">
+        <v>0.19</v>
+      </c>
+      <c r="I52" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>34</v>
+      </c>
+      <c r="L52" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:P39">
-    <sortCondition descending="1" ref="B23:B39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A28:P43">
+    <sortCondition descending="1" ref="B28:B43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed the vapor field equations
</commit_message>
<xml_diff>
--- a/nesh/lambda calculations with revised sigma_m.xlsx
+++ b/nesh/lambda calculations with revised sigma_m.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nesh/Documents/Repositories/icecontinuum/nesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC97A10-DA68-3D43-B464-8165CEEE621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001BDC0F-4E20-5F45-ACC9-EE53E7B9E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="500" windowWidth="26640" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
+    <workbookView xWindow="6900" yWindow="500" windowWidth="21900" windowHeight="15480" xr2:uid="{2DDA9610-AECA-0C43-BEDC-9A13351D73ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>D (um^2/us)</t>
   </si>
@@ -111,6 +111,15 @@
   <si>
     <t>This is the smallest nu_kin I tried</t>
   </si>
+  <si>
+    <t>mc</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>Derived L</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -180,14 +189,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +390,7 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="0.0">
+                <c:pt idx="0">
                   <c:v>9.9469496021220163</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -394,31 +399,31 @@
                 <c:pt idx="2">
                   <c:v>15.789473684210526</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0">
+                <c:pt idx="3">
                   <c:v>4.9570389953734297</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.0">
+                <c:pt idx="4">
                   <c:v>3.0537459283387625</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.0">
+                <c:pt idx="5">
                   <c:v>2.7056277056277058</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.0">
+                <c:pt idx="6">
                   <c:v>22.255192878338278</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.0">
+                <c:pt idx="7">
                   <c:v>31.380753138075313</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.0">
+                <c:pt idx="8">
                   <c:v>5.4744525547445262</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="0.0">
+                <c:pt idx="9">
                   <c:v>3.5561877667140824</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.0">
+                <c:pt idx="10">
                   <c:v>2.6483050847457625</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="0.0">
+                <c:pt idx="11">
                   <c:v>15.306122448979592</c:v>
                 </c:pt>
               </c:numCache>
@@ -527,7 +532,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2108,16 +2113,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1282700</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>363977</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>92029</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>659476</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>184421</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2480,9 +2485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FACA8F-BEA8-A344-9B24-B4206D9D79F6}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B13"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2490,10 +2495,10 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="13"/>
+    <col min="4" max="4" width="10.83203125" style="8"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="8" customWidth="1"/>
     <col min="11" max="12" width="13.33203125" customWidth="1"/>
     <col min="13" max="13" width="16.5" customWidth="1"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
@@ -2509,7 +2514,7 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -2518,7 +2523,7 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
@@ -2533,26 +2538,29 @@
       <c r="K1" t="s">
         <v>13</v>
       </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B2" s="9">
+      <c r="B2" s="3">
         <f>F2^$C$19*C2^$C$22*K2^$C$21*I2^$C$20*10</f>
         <v>1.0846522890932808</v>
       </c>
       <c r="C2">
         <v>75</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="10">
         <v>7.54</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f t="shared" ref="E2" si="0">C2/D2</f>
         <v>9.9469496021220163</v>
       </c>
       <c r="F2" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="9">
         <v>0.22</v>
       </c>
       <c r="H2">
@@ -2561,32 +2569,36 @@
       <c r="I2" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="N2" s="7">
+        <f>(I2*100-$G$20)/$G$19</f>
+        <v>16.127819548872182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
         <f>F3^$C$19*C3^$C$22*K3^$C$21*I3^$C$20*10</f>
         <v>0.76696498884737041</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3">
         <v>75</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="10">
         <v>10.77</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="4">
         <f t="shared" ref="E3:E5" si="1">C3/D3</f>
         <v>6.9637883008356551</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="9">
         <v>0.22</v>
       </c>
       <c r="H3">
@@ -2595,69 +2607,77 @@
       <c r="I3" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3">
         <v>34</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
+      <c r="N3" s="7">
+        <f t="shared" ref="N3:N13" si="2">(I3*100-$G$20)/$G$19</f>
+        <v>25.526315789473689</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <f>F4^$C$19*C4^$C$22*K4^$C$21*I4^$C$20*10</f>
         <v>1.7149858514250884</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4">
         <v>75</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="10">
         <v>4.75</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="4">
         <f t="shared" si="1"/>
         <v>15.789473684210526</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="9">
         <v>0.22</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4">
         <v>0.2</v>
       </c>
       <c r="I4" s="6">
         <v>1E-3</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4">
         <v>34</v>
       </c>
+      <c r="N4" s="7">
+        <f t="shared" si="2"/>
+        <v>10.488721804511279</v>
+      </c>
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <f t="shared" ref="B5" si="2">F5^$C$19*C5^$C$22*K5^$C$21*I5^$C$20*10</f>
+      <c r="B5" s="3">
+        <f t="shared" ref="B5" si="3">F5^$C$19*C5^$C$22*K5^$C$21*I5^$C$20*10</f>
         <v>0.54232614454664041</v>
       </c>
       <c r="C5">
         <v>75</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="10">
         <v>15.13</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f t="shared" si="1"/>
         <v>4.9570389953734297</v>
       </c>
       <c r="F5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="9">
         <v>0.22</v>
       </c>
       <c r="H5">
@@ -2666,109 +2686,121 @@
       <c r="I5" s="1">
         <v>1E-3</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5">
         <v>34</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" t="s">
         <v>20</v>
+      </c>
+      <c r="N5" s="7">
+        <f t="shared" si="2"/>
+        <v>10.488721804511279</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <f t="shared" ref="B6" si="3">F6^$C$19*C6^$C$22*K6^$C$21*I6^$C$20*10</f>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <f t="shared" ref="B6" si="4">F6^$C$19*C6^$C$22*K6^$C$21*I6^$C$20*10</f>
         <v>0.34299717028501764</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>75</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="10">
         <v>24.56</v>
       </c>
-      <c r="E6" s="11">
-        <f t="shared" ref="E6" si="4">C6/D6</f>
+      <c r="E6" s="4">
+        <f t="shared" ref="E6" si="5">C6/D6</f>
         <v>3.0537459283387625</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="9">
         <v>0.22</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6">
         <v>0.2</v>
       </c>
       <c r="I6" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
-        <f t="shared" ref="B7:B8" si="5">F7^$C$19*C7^$C$22*K7^$C$21*I7^$C$20*10</f>
+      <c r="N6" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <f t="shared" ref="B7:B8" si="6">F7^$C$19*C7^$C$22*K7^$C$21*I7^$C$20*10</f>
         <v>0.30678599553894814</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>75</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="10">
         <v>27.72</v>
       </c>
-      <c r="E7" s="11">
-        <f t="shared" ref="E7:E8" si="6">C7/D7</f>
+      <c r="E7" s="4">
+        <f t="shared" ref="E7:E8" si="7">C7/D7</f>
         <v>2.7056277056277058</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="2">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="9">
         <v>0.22</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7">
         <v>0.2</v>
       </c>
       <c r="I7" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7">
         <v>34</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" t="s">
         <v>19</v>
       </c>
+      <c r="N7" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
     </row>
     <row r="8" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
-        <f t="shared" si="5"/>
+      <c r="B8" s="3">
+        <f t="shared" si="6"/>
         <v>2.4253562503633295</v>
       </c>
       <c r="C8">
         <v>75</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="10">
         <v>3.37</v>
       </c>
-      <c r="E8" s="5">
-        <f t="shared" si="6"/>
+      <c r="E8" s="4">
+        <f t="shared" si="7"/>
         <v>22.255192878338278</v>
       </c>
       <c r="F8" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="9">
         <v>0.22</v>
       </c>
       <c r="H8">
@@ -2777,35 +2809,39 @@
       <c r="I8" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8">
         <v>34</v>
+      </c>
+      <c r="N8" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
-        <f t="shared" ref="B9:B10" si="7">F9^$C$19*C9^$C$22*K9^$C$21*I9^$C$20*10</f>
+      <c r="B9" s="3">
+        <f t="shared" ref="B9:B10" si="8">F9^$C$19*C9^$C$22*K9^$C$21*I9^$C$20*10</f>
         <v>3.4299717028501764</v>
       </c>
       <c r="C9">
         <v>75</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="10">
         <v>2.39</v>
       </c>
-      <c r="E9" s="5">
-        <f t="shared" ref="E9:E10" si="8">C9/D9</f>
+      <c r="E9" s="4">
+        <f t="shared" ref="E9:E10" si="9">C9/D9</f>
         <v>31.380753138075313</v>
       </c>
       <c r="F9" s="2">
         <v>0.01</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="9">
         <v>0.22</v>
       </c>
       <c r="H9">
@@ -2814,35 +2850,39 @@
       <c r="I9" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <v>34</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" t="s">
         <v>23</v>
       </c>
+      <c r="N9" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <f t="shared" si="7"/>
+      <c r="B10" s="3">
+        <f t="shared" si="8"/>
         <v>0.63245553203367577</v>
       </c>
       <c r="C10">
         <v>75</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>13.7</v>
       </c>
-      <c r="E10" s="5">
-        <f t="shared" si="8"/>
+      <c r="E10" s="4">
+        <f t="shared" si="9"/>
         <v>5.4744525547445262</v>
       </c>
       <c r="F10" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="9">
         <v>0.22</v>
       </c>
       <c r="H10">
@@ -2851,32 +2891,36 @@
       <c r="I10" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <v>100</v>
       </c>
+      <c r="N10" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
     </row>
     <row r="11" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
-        <f t="shared" ref="B11" si="9">F11^$C$19*C11^$C$22*K11^$C$21*I11^$C$20*10</f>
+      <c r="B11" s="3">
+        <f t="shared" ref="B11" si="10">F11^$C$19*C11^$C$22*K11^$C$21*I11^$C$20*10</f>
         <v>0.44721359549995787</v>
       </c>
       <c r="C11">
         <v>75</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <v>21.09</v>
       </c>
-      <c r="E11" s="5">
-        <f t="shared" ref="E11" si="10">C11/D11</f>
+      <c r="E11" s="4">
+        <f t="shared" ref="E11" si="11">C11/D11</f>
         <v>3.5561877667140824</v>
       </c>
       <c r="F11" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="9">
         <v>0.22</v>
       </c>
       <c r="H11">
@@ -2885,32 +2929,36 @@
       <c r="I11" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11">
         <v>200</v>
       </c>
+      <c r="N11" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
     </row>
     <row r="12" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
-        <f t="shared" ref="B12" si="11">F12^$C$19*C12^$C$22*K12^$C$21*I12^$C$20*10</f>
+      <c r="B12" s="3">
+        <f t="shared" ref="B12" si="12">F12^$C$19*C12^$C$22*K12^$C$21*I12^$C$20*10</f>
         <v>0.36514837167011066</v>
       </c>
       <c r="C12">
         <v>75</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="10">
         <v>28.32</v>
       </c>
-      <c r="E12" s="5">
-        <f t="shared" ref="E12" si="12">C12/D12</f>
+      <c r="E12" s="4">
+        <f t="shared" ref="E12" si="13">C12/D12</f>
         <v>2.6483050847457625</v>
       </c>
       <c r="F12" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="9">
         <v>0.22</v>
       </c>
       <c r="H12">
@@ -2919,35 +2967,39 @@
       <c r="I12" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12">
         <v>300</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" t="s">
         <v>21</v>
       </c>
+      <c r="N12" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
     </row>
     <row r="13" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
-        <f t="shared" ref="B13" si="13">F13^$C$19*C13^$C$22*K13^$C$21*I13^$C$20*10</f>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13" si="14">F13^$C$19*C13^$C$22*K13^$C$21*I13^$C$20*10</f>
         <v>1.6329931618554518</v>
       </c>
       <c r="C13">
         <v>75</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E13" s="5">
-        <f t="shared" ref="E13" si="14">C13/D13</f>
+      <c r="E13" s="4">
+        <f t="shared" ref="E13" si="15">C13/D13</f>
         <v>15.306122448979592</v>
       </c>
       <c r="F13" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="9">
         <v>0.22</v>
       </c>
       <c r="H13">
@@ -2956,74 +3008,78 @@
       <c r="I13" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13">
         <v>15</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" t="s">
         <v>24</v>
       </c>
+      <c r="N13" s="7">
+        <f t="shared" si="2"/>
+        <v>16.127819548872182</v>
+      </c>
     </row>
     <row r="14" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
+      <c r="B14" s="3"/>
       <c r="C14"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="9"/>
       <c r="H14"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
     </row>
     <row r="15" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
+      <c r="B15" s="3"/>
       <c r="C15"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="9"/>
       <c r="H15"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
     </row>
     <row r="16" spans="1:16" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+      <c r="B16" s="3"/>
       <c r="C16"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="5"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="14"/>
+      <c r="G16" s="9"/>
       <c r="H16"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
     </row>
     <row r="17" spans="2:12" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
+      <c r="B17" s="3"/>
       <c r="C17"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="9"/>
       <c r="H17"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
     </row>
     <row r="18" spans="2:12" ht="17" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="9"/>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:12" ht="17" x14ac:dyDescent="0.25">
@@ -3033,10 +3089,14 @@
       <c r="C19">
         <v>0.5</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="11">
+        <v>2.6599999999999999E-2</v>
+      </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -3046,6 +3106,12 @@
       <c r="C20">
         <v>-0.5</v>
       </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="8">
+        <v>-0.17899999999999999</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -3068,263 +3134,263 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B28" s="9">
-        <f t="shared" ref="B28:B44" si="15">G28</f>
+    <row r="28" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <f t="shared" ref="B28:B44" si="16">G28</f>
         <v>0.7</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28">
         <v>75</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="10">
         <v>27.87</v>
       </c>
-      <c r="E28" s="10">
-        <f t="shared" ref="E28:E44" si="16">C28/D28</f>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:E44" si="17">C28/D28</f>
         <v>2.6910656620021527</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="9">
         <v>0.7</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28">
         <v>0.2</v>
       </c>
       <c r="I28" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J28">
         <v>1</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B29" s="9">
-        <f t="shared" si="15"/>
+    <row r="29" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29">
         <v>75</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="10">
         <v>22.86</v>
       </c>
-      <c r="E29" s="10">
-        <f t="shared" si="16"/>
+      <c r="E29" s="4">
+        <f t="shared" si="17"/>
         <v>3.2808398950131235</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="9">
         <v>0.6</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29">
         <v>0.2</v>
       </c>
       <c r="I29" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29">
         <v>1</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B30" s="9">
-        <f t="shared" si="15"/>
+    <row r="30" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
+        <f t="shared" si="16"/>
         <v>0.4</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30">
         <v>75</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="10">
         <v>13.97</v>
       </c>
-      <c r="E30" s="10">
-        <f t="shared" si="16"/>
+      <c r="E30" s="4">
+        <f t="shared" si="17"/>
         <v>5.3686471009305654</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="9">
         <v>0.4</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30">
         <v>0.2</v>
       </c>
       <c r="I30" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30">
         <v>1</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B31" s="9">
-        <f t="shared" si="15"/>
+    <row r="31" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <f t="shared" si="16"/>
         <v>0.3</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31">
         <v>75</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="10">
         <v>9.9700000000000006</v>
       </c>
-      <c r="E31" s="10">
-        <f t="shared" si="16"/>
+      <c r="E31" s="4">
+        <f t="shared" si="17"/>
         <v>7.5225677031093277</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="9">
         <v>0.3</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31">
         <v>0.2</v>
       </c>
       <c r="I31" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J31" s="8">
+      <c r="J31">
         <v>1</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="2:12" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B32" s="9">
-        <f t="shared" si="15"/>
+    <row r="32" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <f t="shared" si="16"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32">
         <v>75</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="10">
         <v>9.0399999999999991</v>
       </c>
-      <c r="E32" s="10">
-        <f t="shared" si="16"/>
+      <c r="E32" s="4">
+        <f t="shared" si="17"/>
         <v>8.2964601769911503</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="9">
         <v>0.27500000000000002</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32">
         <v>0.2</v>
       </c>
       <c r="I32" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J32" s="8">
+      <c r="J32">
         <v>1</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B33" s="9">
-        <f t="shared" si="15"/>
+    <row r="33" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <f t="shared" si="16"/>
         <v>0.25</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33">
         <v>75</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="10">
         <v>8.18</v>
       </c>
-      <c r="E33" s="10">
-        <f t="shared" si="16"/>
+      <c r="E33" s="4">
+        <f t="shared" si="17"/>
         <v>9.1687041564792171</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="9">
         <v>0.25</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33">
         <v>0.2</v>
       </c>
       <c r="I33" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33">
         <v>1</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B34" s="9">
-        <f t="shared" si="15"/>
+    <row r="34" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <f t="shared" si="16"/>
         <v>0.23</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34">
         <v>75</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="10">
         <v>7.65</v>
       </c>
-      <c r="E34" s="10">
-        <f t="shared" si="16"/>
+      <c r="E34" s="4">
+        <f t="shared" si="17"/>
         <v>9.8039215686274499</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="9">
         <v>0.23</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34">
         <v>0.2</v>
       </c>
       <c r="I34" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J34" s="8">
+      <c r="J34">
         <v>1</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="17" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.22</v>
       </c>
       <c r="C35">
         <v>75</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="10">
         <v>7.54</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9469496021220163</v>
       </c>
       <c r="F35" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="9">
         <v>0.22</v>
       </c>
       <c r="H35">
@@ -3340,300 +3406,300 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B36" s="9">
-        <f t="shared" si="15"/>
+    <row r="36" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <f t="shared" si="16"/>
         <v>0.21</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36">
         <v>75</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="10">
         <v>7.83</v>
       </c>
-      <c r="E36" s="10">
-        <f t="shared" si="16"/>
+      <c r="E36" s="4">
+        <f t="shared" si="17"/>
         <v>9.5785440613026811</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="9">
         <v>0.21</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36">
         <v>0.2</v>
       </c>
       <c r="I36" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J36" s="8">
+      <c r="J36">
         <v>1</v>
       </c>
-      <c r="K36" s="8">
+      <c r="K36">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B37" s="9">
-        <f t="shared" si="15"/>
+    <row r="37" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <f t="shared" si="16"/>
         <v>-0.02</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37">
         <v>75</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="10">
         <v>2.2599999999999998</v>
       </c>
-      <c r="E37" s="10">
-        <f t="shared" si="16"/>
+      <c r="E37" s="4">
+        <f t="shared" si="17"/>
         <v>33.185840707964601</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="9">
         <v>-0.02</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37">
         <v>0.2</v>
       </c>
       <c r="I37" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J37" s="8">
+      <c r="J37">
         <v>1</v>
       </c>
-      <c r="K37" s="8">
+      <c r="K37">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B38" s="9">
-        <f t="shared" si="15"/>
+    <row r="38" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <f t="shared" si="16"/>
         <v>-0.03</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38">
         <v>75</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="10">
         <v>2.75</v>
       </c>
-      <c r="E38" s="10">
-        <f t="shared" si="16"/>
+      <c r="E38" s="4">
+        <f t="shared" si="17"/>
         <v>27.272727272727273</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F38" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="9">
         <v>-0.03</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38">
         <v>0.2</v>
       </c>
       <c r="I38" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J38" s="8">
+      <c r="J38">
         <v>1</v>
       </c>
-      <c r="K38" s="8">
+      <c r="K38">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B39" s="9">
-        <f t="shared" si="15"/>
+    <row r="39" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <f t="shared" si="16"/>
         <v>-0.05</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39">
         <v>75</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="10">
         <v>3.66</v>
       </c>
-      <c r="E39" s="10">
-        <f t="shared" si="16"/>
+      <c r="E39" s="4">
+        <f t="shared" si="17"/>
         <v>20.491803278688522</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="9">
         <v>-0.05</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39">
         <v>0.2</v>
       </c>
       <c r="I39" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39">
         <v>1</v>
       </c>
-      <c r="K39" s="8">
+      <c r="K39">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B40" s="9">
-        <f t="shared" si="15"/>
+    <row r="40" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <f t="shared" si="16"/>
         <v>-0.1</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40">
         <v>75</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="10">
         <v>5.73</v>
       </c>
-      <c r="E40" s="10">
-        <f t="shared" si="16"/>
+      <c r="E40" s="4">
+        <f t="shared" si="17"/>
         <v>13.089005235602093</v>
       </c>
-      <c r="F40" s="12">
+      <c r="F40" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="9">
         <v>-0.1</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40">
         <v>0.2</v>
       </c>
       <c r="I40" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J40" s="8">
+      <c r="J40">
         <v>1</v>
       </c>
-      <c r="K40" s="8">
+      <c r="K40">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B41" s="9">
-        <f t="shared" si="15"/>
+    <row r="41" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <f t="shared" si="16"/>
         <v>-0.2</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41">
         <v>75</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="10">
         <v>9.76</v>
       </c>
-      <c r="E41" s="10">
-        <f t="shared" si="16"/>
+      <c r="E41" s="4">
+        <f t="shared" si="17"/>
         <v>7.6844262295081966</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="9">
         <v>-0.2</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41">
         <v>0.2</v>
       </c>
       <c r="I41" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J41" s="8">
+      <c r="J41">
         <v>1</v>
       </c>
-      <c r="K41" s="8">
+      <c r="K41">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B42" s="9">
-        <f t="shared" si="15"/>
+    <row r="42" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <f t="shared" si="16"/>
         <v>-0.3</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42">
         <v>75</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="10">
         <v>13.96</v>
       </c>
-      <c r="E42" s="10">
-        <f t="shared" si="16"/>
+      <c r="E42" s="4">
+        <f t="shared" si="17"/>
         <v>5.3724928366762175</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="9">
         <v>-0.3</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42">
         <v>0.2</v>
       </c>
       <c r="I42" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J42" s="8">
+      <c r="J42">
         <v>1</v>
       </c>
-      <c r="K42" s="8">
+      <c r="K42">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B43" s="9">
-        <f t="shared" si="15"/>
+    <row r="43" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <f t="shared" si="16"/>
         <v>-0.4</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43">
         <v>75</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="10">
         <v>18.38</v>
       </c>
-      <c r="E43" s="10">
-        <f t="shared" si="16"/>
+      <c r="E43" s="4">
+        <f t="shared" si="17"/>
         <v>4.0805223068552774</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="9">
         <v>-0.4</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43">
         <v>0.2</v>
       </c>
       <c r="I43" s="1">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J43" s="8">
+      <c r="J43">
         <v>1</v>
       </c>
-      <c r="K43" s="8">
+      <c r="K43">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:11" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="B44" s="9">
-        <f t="shared" si="15"/>
+    <row r="44" spans="2:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <f t="shared" si="16"/>
         <v>-0.5</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44">
         <v>76</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="10">
         <v>23.11</v>
       </c>
-      <c r="E44" s="10">
-        <f t="shared" si="16"/>
+      <c r="E44" s="4">
+        <f t="shared" si="17"/>
         <v>3.288619645175249</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="9">
         <v>-0.5</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H44">
         <v>0.2</v>
       </c>
       <c r="I44" s="1">
@@ -3642,10 +3708,10 @@
     </row>
     <row r="45" spans="2:11" ht="17" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
-      <c r="D45" s="15"/>
+      <c r="D45" s="10"/>
       <c r="E45" s="5"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="14"/>
+      <c r="G45" s="9"/>
       <c r="I45" s="1"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
@@ -3660,7 +3726,7 @@
       <c r="F48" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="8">
         <v>0.19400000000000001</v>
       </c>
       <c r="H48">
@@ -3684,7 +3750,7 @@
       <c r="F49" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="8">
         <v>0.192</v>
       </c>
       <c r="H49">
@@ -3705,12 +3771,12 @@
       <c r="C50">
         <v>75</v>
       </c>
-      <c r="D50" s="15"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="5"/>
       <c r="F50" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G50" s="9">
         <v>-0.5</v>
       </c>
       <c r="H50">
@@ -3731,12 +3797,12 @@
       <c r="C51">
         <v>75</v>
       </c>
-      <c r="D51" s="15"/>
+      <c r="D51" s="10"/>
       <c r="E51" s="5"/>
       <c r="F51" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="9">
         <v>0.19500000000000001</v>
       </c>
       <c r="H51">
@@ -3757,7 +3823,7 @@
       <c r="C52">
         <v>75</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="10">
         <v>6.91</v>
       </c>
       <c r="E52" s="5">
@@ -3767,7 +3833,7 @@
       <c r="F52" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="9">
         <v>0.2</v>
       </c>
       <c r="H52">

</xml_diff>